<commit_message>
datafile and login TC changes
</commit_message>
<xml_diff>
--- a/KISANCHAT-25-04-2018/src/test/java/TestData/ExcelData.xlsx
+++ b/KISANCHAT-25-04-2018/src/test/java/TestData/ExcelData.xlsx
@@ -5,11 +5,12 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="Channel" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="MyChatList" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="19">
   <si>
     <t xml:space="preserve">Mobile Number</t>
   </si>
@@ -75,6 +76,9 @@
   </si>
   <si>
     <t xml:space="preserve">#11ee62</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Channel 92</t>
   </si>
 </sst>
 </file>
@@ -131,7 +135,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
+  <cellStyleXfs count="21">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -155,44 +159,49 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellStyleXfs>
   <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="20" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="20" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="20" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
-  <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+  <cellStyles count="7">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5"/>
+    <cellStyle name="Excel Built-in Normal" xfId="20"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -268,15 +277,16 @@
       <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="14.65" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="21.82"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="20.98"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="25.56"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="4" style="2" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="20.97"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="25.55"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="257" min="4" style="2" width="11.51"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="258" style="0" width="11.51"/>
   </cols>
   <sheetData>
-    <row r="1" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" s="4" customFormat="true" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -287,7 +297,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="n">
         <v>9403247980</v>
       </c>
@@ -298,7 +308,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="n">
         <v>7350368582</v>
       </c>
@@ -325,66 +335,103 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:I3"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.65" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="5" width="14.02"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="5" width="13.74"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="5" width="14.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="5" width="13.46"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="7" min="5" style="5" width="11.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="5" width="15.55"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="257" min="9" style="5" width="11.51"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="258" style="0" width="11.51"/>
+  </cols>
+  <sheetData>
+    <row r="1" s="6" customFormat="true" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="I1" s="6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F13" activeCellId="0" sqref="F13"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="14.65" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="5" width="14.03"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="5" width="13.75"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="5" width="14.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="5" width="13.47"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="7" min="5" style="5" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="5" width="15.56"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="9" style="5" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="26.12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="34.87"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="8.67"/>
   </cols>
   <sheetData>
-    <row r="1" s="6" customFormat="true" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="B1" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C1" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="D1" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E1" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="F1" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="G1" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="H1" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="I1" s="6" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>17</v>
-      </c>
-    </row>
+    <row r="1" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="2" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
login and Listchannels TC working with data write in excel file
</commit_message>
<xml_diff>
--- a/KISANCHAT-25-04-2018/src/test/java/TestData/ExcelData.xlsx
+++ b/KISANCHAT-25-04-2018/src/test/java/TestData/ExcelData.xlsx
@@ -274,7 +274,7 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A:A"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.65" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -338,7 +338,7 @@
   <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A:A"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.65" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -420,18 +420,42 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A:A"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.65" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="26.12"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="34.87"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="7.36"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="77.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="8.67"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="2" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
Exhibitor Login TC completed
</commit_message>
<xml_diff>
--- a/KISANCHAT-25-04-2018/src/test/java/TestData/ExcelData.xlsx
+++ b/KISANCHAT-25-04-2018/src/test/java/TestData/ExcelData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="24">
   <si>
     <t xml:space="preserve">Mobile Number</t>
   </si>
@@ -33,10 +33,25 @@
     <t xml:space="preserve">UserLastName</t>
   </si>
   <si>
+    <t xml:space="preserve">Exhibitor Username</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Exhibitor Password</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Exhibitor Mobile Number</t>
+  </si>
+  <si>
     <t xml:space="preserve">Chetan</t>
   </si>
   <si>
     <t xml:space="preserve">Warke</t>
+  </si>
+  <si>
+    <t xml:space="preserve">exh_0006@mailinator.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">chan@kisan18</t>
   </si>
   <si>
     <t xml:space="preserve">Channel Name</t>
@@ -89,7 +104,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="#"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -111,6 +126,27 @@
       <name val="Arial"/>
       <family val="0"/>
     </font>
+    <font>
+      <sz val="13"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="13"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="13"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -126,7 +162,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -134,6 +170,13 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="hair"/>
+      <right style="hair"/>
+      <top style="hair"/>
+      <bottom style="hair"/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="21">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
@@ -164,25 +207,45 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="12">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="20" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="20" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="2" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="2" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="2" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="20" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -271,55 +334,217 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:G20"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A:A"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.65" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="16.15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="21.82"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="20.97"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="25.55"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="257" min="4" style="2" width="11.51"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="258" style="0" width="11.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="18.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="18.24"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="11.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="32.09"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="2" width="23.94"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="2" width="31.16"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="257" min="8" style="2" width="11.51"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="258" style="3" width="11.51"/>
   </cols>
   <sheetData>
-    <row r="1" s="4" customFormat="true" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="3" t="s">
+    <row r="1" s="6" customFormat="true" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="5" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="n">
+      <c r="E1" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="7" t="n">
         <v>9403247980</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="n">
+      <c r="B2" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="G2" s="8"/>
+    </row>
+    <row r="3" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="7" t="n">
         <v>7350368582</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>4</v>
-      </c>
+      <c r="B3" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" s="8"/>
+      <c r="F3" s="8"/>
+      <c r="G3" s="8"/>
+    </row>
+    <row r="4" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="7"/>
+      <c r="B4" s="8"/>
+      <c r="C4" s="8"/>
+      <c r="E4" s="8"/>
+      <c r="F4" s="8"/>
+      <c r="G4" s="8"/>
+    </row>
+    <row r="5" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="7"/>
+      <c r="B5" s="8"/>
+      <c r="C5" s="8"/>
+      <c r="E5" s="8"/>
+      <c r="F5" s="8"/>
+      <c r="G5" s="8"/>
+    </row>
+    <row r="6" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="7"/>
+      <c r="B6" s="8"/>
+      <c r="C6" s="8"/>
+      <c r="E6" s="8"/>
+      <c r="F6" s="8"/>
+      <c r="G6" s="8"/>
+    </row>
+    <row r="7" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="7"/>
+      <c r="B7" s="8"/>
+      <c r="C7" s="8"/>
+      <c r="E7" s="8"/>
+      <c r="F7" s="8"/>
+      <c r="G7" s="8"/>
+    </row>
+    <row r="8" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="7"/>
+      <c r="B8" s="8"/>
+      <c r="C8" s="8"/>
+      <c r="E8" s="8"/>
+      <c r="F8" s="8"/>
+      <c r="G8" s="8"/>
+    </row>
+    <row r="9" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="7"/>
+      <c r="B9" s="8"/>
+      <c r="C9" s="8"/>
+      <c r="E9" s="8"/>
+      <c r="F9" s="8"/>
+      <c r="G9" s="8"/>
+    </row>
+    <row r="10" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="7"/>
+      <c r="B10" s="8"/>
+      <c r="C10" s="8"/>
+      <c r="E10" s="8"/>
+      <c r="F10" s="8"/>
+      <c r="G10" s="8"/>
+    </row>
+    <row r="11" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="7"/>
+      <c r="B11" s="8"/>
+      <c r="C11" s="8"/>
+      <c r="E11" s="8"/>
+      <c r="F11" s="8"/>
+      <c r="G11" s="8"/>
+    </row>
+    <row r="12" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="7"/>
+      <c r="B12" s="8"/>
+      <c r="C12" s="8"/>
+      <c r="E12" s="8"/>
+      <c r="F12" s="8"/>
+      <c r="G12" s="8"/>
+    </row>
+    <row r="13" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="7"/>
+      <c r="B13" s="8"/>
+      <c r="C13" s="8"/>
+      <c r="E13" s="8"/>
+      <c r="F13" s="8"/>
+      <c r="G13" s="8"/>
+    </row>
+    <row r="14" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="7"/>
+      <c r="B14" s="8"/>
+      <c r="C14" s="8"/>
+      <c r="E14" s="8"/>
+      <c r="F14" s="8"/>
+      <c r="G14" s="8"/>
+    </row>
+    <row r="15" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="7"/>
+      <c r="B15" s="8"/>
+      <c r="C15" s="8"/>
+      <c r="E15" s="8"/>
+      <c r="F15" s="8"/>
+      <c r="G15" s="8"/>
+    </row>
+    <row r="16" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="7"/>
+      <c r="B16" s="8"/>
+      <c r="C16" s="8"/>
+      <c r="E16" s="8"/>
+      <c r="F16" s="8"/>
+      <c r="G16" s="8"/>
+    </row>
+    <row r="17" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="7"/>
+      <c r="B17" s="8"/>
+      <c r="C17" s="8"/>
+      <c r="E17" s="8"/>
+      <c r="F17" s="8"/>
+      <c r="G17" s="8"/>
+    </row>
+    <row r="18" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="7"/>
+      <c r="B18" s="8"/>
+      <c r="C18" s="8"/>
+      <c r="E18" s="8"/>
+      <c r="F18" s="8"/>
+      <c r="G18" s="8"/>
+    </row>
+    <row r="19" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="7"/>
+      <c r="B19" s="8"/>
+      <c r="C19" s="8"/>
+      <c r="E19" s="8"/>
+      <c r="F19" s="8"/>
+      <c r="G19" s="8"/>
+    </row>
+    <row r="20" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="7"/>
+      <c r="B20" s="8"/>
+      <c r="C20" s="8"/>
+      <c r="E20" s="8"/>
+      <c r="F20" s="8"/>
+      <c r="G20" s="8"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E2" r:id="rId1" display="exh_0006@mailinator.com"/>
+  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -338,67 +563,67 @@
   <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A:A"/>
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.65" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="5" width="14.02"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="5" width="13.74"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="5" width="14.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="5" width="13.46"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="7" min="5" style="5" width="11.51"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="5" width="15.55"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="257" min="9" style="5" width="11.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="10" width="14.02"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="10" width="13.74"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="10" width="14.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="10" width="13.46"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="7" min="5" style="10" width="11.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="10" width="15.55"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="257" min="9" style="10" width="11.51"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="258" style="0" width="11.51"/>
   </cols>
   <sheetData>
-    <row r="1" s="6" customFormat="true" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="B1" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C1" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="D1" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E1" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="F1" s="6" t="s">
+    <row r="1" s="11" customFormat="true" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="B1" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="C1" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="D1" s="11" t="s">
         <v>13</v>
       </c>
+      <c r="E1" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="H1" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="I1" s="11" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>17</v>
+      <c r="A2" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="5" t="s">
-        <v>18</v>
+      <c r="A3" s="10" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -419,8 +644,8 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A:A"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.65" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
Search channel from discover changes
</commit_message>
<xml_diff>
--- a/KISANCHAT-25-04-2018/src/test/java/TestData/ExcelData.xlsx
+++ b/KISANCHAT-25-04-2018/src/test/java/TestData/ExcelData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="27">
   <si>
     <t xml:space="preserve">Mobile Number</t>
   </si>
@@ -46,6 +46,12 @@
   </si>
   <si>
     <t xml:space="preserve">Warke</t>
+  </si>
+  <si>
+    <t xml:space="preserve">manisha.kisan17@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">manisha123</t>
   </si>
   <si>
     <t xml:space="preserve">exh_0006@mailinator.com</t>
@@ -107,7 +113,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="#"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -150,6 +156,13 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <b val="true"/>
+      <sz val="13"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -210,7 +223,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -248,6 +261,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="6" fillId="0" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -339,8 +356,8 @@
   </sheetPr>
   <dimension ref="A1:G20"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F14" activeCellId="0" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -404,8 +421,12 @@
       <c r="C3" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="8"/>
-      <c r="F3" s="8"/>
+      <c r="E3" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" s="10" t="s">
+        <v>11</v>
+      </c>
       <c r="G3" s="8"/>
     </row>
     <row r="4" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -546,7 +567,9 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" display="exh_0006@mailinator.com"/>
+    <hyperlink ref="E2" r:id="rId1" display="manisha.kisan17@gmail.com"/>
+    <hyperlink ref="E3" r:id="rId2" display="exh_0006@mailinator.com"/>
+    <hyperlink ref="F3" r:id="rId3" display="chan@kisan18"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -565,73 +588,73 @@
   </sheetPr>
   <dimension ref="A1:I4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E12" activeCellId="0" sqref="E12"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.65" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="10" width="14.02"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="10" width="13.74"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="10" width="14.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="10" width="13.46"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="7" min="5" style="10" width="11.51"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="10" width="15.55"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="257" min="9" style="10" width="11.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="11" width="14.02"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="11" width="13.74"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="11" width="14.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="11" width="13.46"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="7" min="5" style="11" width="11.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="11" width="15.55"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="257" min="9" style="11" width="11.51"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="258" style="0" width="11.51"/>
   </cols>
   <sheetData>
-    <row r="1" s="11" customFormat="true" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="B1" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="C1" s="11" t="s">
+    <row r="1" s="12" customFormat="true" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="11" t="s">
+      <c r="B1" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="E1" s="11" t="s">
+      <c r="C1" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="F1" s="11" t="s">
+      <c r="D1" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="G1" s="11" t="s">
+      <c r="E1" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="H1" s="11" t="s">
+      <c r="F1" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="I1" s="11" t="s">
+      <c r="G1" s="12" t="s">
         <v>18</v>
       </c>
+      <c r="H1" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="I1" s="12" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="B2" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="C2" s="10" t="s">
+      <c r="A2" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="D2" s="10" t="s">
+      <c r="B2" s="11" t="s">
         <v>22</v>
       </c>
+      <c r="C2" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="10" t="s">
-        <v>23</v>
+      <c r="A3" s="11" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="10" t="s">
-        <v>24</v>
+      <c r="A4" s="11" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
wait for loader in baseclass added
</commit_message>
<xml_diff>
--- a/KISANCHAT-25-04-2018/src/test/java/TestData/ExcelData.xlsx
+++ b/KISANCHAT-25-04-2018/src/test/java/TestData/ExcelData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" state="visible" r:id="rId2"/>
@@ -99,7 +99,7 @@
     <t xml:space="preserve">#11ee62</t>
   </si>
   <si>
-    <t xml:space="preserve">Channel 92</t>
+    <t xml:space="preserve">Kisan</t>
   </si>
   <si>
     <t xml:space="preserve">Channel 0007</t>
@@ -113,7 +113,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="#"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -156,13 +156,6 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
-    <font>
-      <b val="true"/>
-      <sz val="13"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -223,7 +216,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -261,10 +254,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="6" fillId="0" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -356,7 +345,7 @@
   </sheetPr>
   <dimension ref="A1:G20"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="F14" activeCellId="0" sqref="F14"/>
     </sheetView>
   </sheetViews>
@@ -421,10 +410,10 @@
       <c r="C3" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="10" t="s">
+      <c r="E3" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="F3" s="10" t="s">
+      <c r="F3" s="9" t="s">
         <v>11</v>
       </c>
       <c r="G3" s="8"/>
@@ -588,72 +577,72 @@
   </sheetPr>
   <dimension ref="A1:I4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.65" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="11" width="14.02"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="11" width="13.74"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="11" width="14.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="11" width="13.46"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="7" min="5" style="11" width="11.51"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="11" width="15.55"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="257" min="9" style="11" width="11.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="10" width="14.02"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="10" width="13.74"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="10" width="14.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="10" width="13.46"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="7" min="5" style="10" width="11.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="10" width="15.55"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="257" min="9" style="10" width="11.51"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="258" style="0" width="11.51"/>
   </cols>
   <sheetData>
-    <row r="1" s="12" customFormat="true" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="12" t="s">
+    <row r="1" s="11" customFormat="true" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="C1" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="D1" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="E1" s="12" t="s">
+      <c r="E1" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="F1" s="12" t="s">
+      <c r="F1" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="G1" s="12" t="s">
+      <c r="G1" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="H1" s="12" t="s">
+      <c r="H1" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="I1" s="12" t="s">
+      <c r="I1" s="11" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="C2" s="11" t="s">
+      <c r="C2" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="D2" s="11" t="s">
+      <c r="D2" s="10" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="11" t="s">
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="10" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="11" t="s">
+      <c r="A4" s="10" t="s">
         <v>26</v>
       </c>
     </row>

</xml_diff>